<commit_message>
ver1.40 Stars in Button Area
</commit_message>
<xml_diff>
--- a/docs/Design.xlsx
+++ b/docs/Design.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\NumNum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\NumNum\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905761D4-DFBA-4203-97DC-1DBE24782FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AEB6B4-9003-4030-85AA-CC7EB28420A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ver1.39" sheetId="1" r:id="rId1"/>
+    <sheet name="ver1.40" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -2766,6 +2766,1708 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>143996</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>65555</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="テキスト ボックス 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17258B4A-3E28-D158-07EC-2F076A5E617A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7705724" y="8802221"/>
+          <a:ext cx="542926" cy="397809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1600" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>466724</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>143996</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>65555</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="テキスト ボックス 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18E68977-FCE5-12D8-B5F2-356AC5F38801}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8010524" y="8802221"/>
+          <a:ext cx="542926" cy="397809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1600" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>143996</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>65555</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="テキスト ボックス 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E23BB142-07E2-AC38-6180-84C7B283A408}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8343899" y="8802221"/>
+          <a:ext cx="542926" cy="397809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1600" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>409574</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>143996</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>65555</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="テキスト ボックス 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BFBD5A7-A03F-37D7-BCFA-F38BA828A8F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8639174" y="8802221"/>
+          <a:ext cx="542926" cy="397809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1600" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>143996</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>65555</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="テキスト ボックス 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DF189CA-39F0-FE6A-FADF-1EC4733CC5E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8953499" y="8802221"/>
+          <a:ext cx="542926" cy="397809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1600" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>361949</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>143996</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>65555</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="テキスト ボックス 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCEF6E5D-BFDB-5938-124A-5F4F3F8B2E62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9277349" y="8802221"/>
+          <a:ext cx="542926" cy="397809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1600" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>143996</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>65555</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="テキスト ボックス 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DB1F1E3-8BF2-27E7-BD6A-86B59C78BF3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9667874" y="8802221"/>
+          <a:ext cx="542926" cy="397809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1600" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>143996</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>65555</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="テキスト ボックス 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F9C2378-B240-B450-07C8-0CC766B49102}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10020299" y="8802221"/>
+          <a:ext cx="542926" cy="397809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1600" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>143996</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>65555</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="テキスト ボックス 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87F417B6-F11E-B18A-0922-0968BD232966}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10334624" y="8802221"/>
+          <a:ext cx="542926" cy="397809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1600" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>390524</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>143996</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>65555</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="テキスト ボックス 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{907E0D40-6CA6-2D7C-F02D-1B807FFF0C3A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10677524" y="8802221"/>
+          <a:ext cx="542926" cy="397809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1600" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>647699</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>143996</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>65555</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="テキスト ボックス 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C39150B-995F-47B6-F118-B8D08E76618C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10934699" y="8802221"/>
+          <a:ext cx="542926" cy="397809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1600" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>228599</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>143996</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>65555</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="テキスト ボックス 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27B6E52E-8388-13D4-5962-CC509DAC3885}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11201399" y="8802221"/>
+          <a:ext cx="542926" cy="397809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1600" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>1121</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>625027</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="テキスト ボックス 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37D43F68-AD75-2780-36E7-FFE13CC35DC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6886574" y="9135596"/>
+          <a:ext cx="596453" cy="437029"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>390524</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>1121</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>301177</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="テキスト ボックス 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFCCA3C2-677C-A584-71DF-1272415D6CAB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7248524" y="9135596"/>
+          <a:ext cx="596453" cy="437029"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>1121</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>682177</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="テキスト ボックス 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74D28890-3219-32FF-0045-17B3D46E10B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7629524" y="9135596"/>
+          <a:ext cx="596453" cy="437029"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457199</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>1121</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>367852</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="テキスト ボックス 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DF4C2AC-5E4E-C570-19D5-17B4D48681ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8000999" y="9135596"/>
+          <a:ext cx="596453" cy="437029"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>1121</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>110677</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="テキスト ボックス 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{031A8D0F-7641-10AD-FD0A-1F79C9EBAF0E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8429624" y="9135596"/>
+          <a:ext cx="596453" cy="437029"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>1121</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>482152</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="テキスト ボックス 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EF0322C-B9CB-EB34-FDE8-F4D30963357A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8801099" y="9135596"/>
+          <a:ext cx="596453" cy="437029"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>1121</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>215452</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="テキスト ボックス 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1DD7B5C-A71B-928F-CB1E-DF2C66A21AE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9220199" y="9135596"/>
+          <a:ext cx="596453" cy="437029"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>1121</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>625027</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="テキスト ボックス 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1755C051-B83C-A14E-60CE-CB23F5B24420}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9629774" y="9135596"/>
+          <a:ext cx="596453" cy="437029"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>485774</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>1121</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>396427</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="テキスト ボックス 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30733274-6A05-57F9-83BC-309B7935D8EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10086974" y="9135596"/>
+          <a:ext cx="596453" cy="437029"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>1121</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>101152</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="テキスト ボックス 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{771391C0-A3F3-A8D7-A153-9B11F589E34D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10477499" y="9135596"/>
+          <a:ext cx="596453" cy="437029"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>1121</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>596452</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="テキスト ボックス 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0DCB1D0-6284-CDD3-8764-F92D1CFF570A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10972799" y="9135596"/>
+          <a:ext cx="596453" cy="437029"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>★</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3035,7 +4737,7 @@
   <dimension ref="B8:K8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X32" sqref="X32"/>
+      <selection activeCell="U38" sqref="U38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>

</xml_diff>